<commit_message>
Ajuste en Jdbc.class de censuses  para las pruebas
</commit_message>
<xml_diff>
--- a/censuses_3b/src/test/resources/test.xlsx
+++ b/censuses_3b/src/test/resources/test.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8370" windowHeight="2370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11370" windowHeight="3690"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Nombre</t>
   </si>
@@ -58,13 +59,16 @@
   </si>
   <si>
     <t>ana@gmail.com</t>
+  </si>
+  <si>
+    <t>AST001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,26 +385,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -424,11 +428,11 @@
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
-        <v>234</v>
+      <c r="D2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -438,11 +442,11 @@
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3">
-        <v>345</v>
+      <c r="D3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -452,8 +456,8 @@
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4">
-        <v>456</v>
+      <c r="D4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pasan los tests de censuses y voters
</commit_message>
<xml_diff>
--- a/censuses_3b/src/test/resources/test.xlsx
+++ b/censuses_3b/src/test/resources/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11370" windowHeight="3690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9675" windowHeight="3690"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Nombre</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>AST001</t>
+  </si>
+  <si>
+    <t>Pepe</t>
+  </si>
+  <si>
+    <t>56982000R</t>
+  </si>
+  <si>
+    <t>pepe@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -393,15 +402,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -457,6 +467,20 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -465,8 +489,9 @@
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>